<commit_message>
CAN1-78 Addressed v1 Comments for Top Module Test Cases --Antonio
</commit_message>
<xml_diff>
--- a/Documentations/Test Cases/top_module_test_cases.xlsx
+++ b/Documentations/Test Cases/top_module_test_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\God\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F05F4EC-C4C4-40AC-B09C-9A7F99E90920}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C644C21-2CE2-4D86-9F9E-0F213629FF9B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD364520-9B66-417D-B195-925AAF6E8BA3}"/>
+    <workbookView xWindow="-8070" yWindow="4665" windowWidth="17055" windowHeight="11385" xr2:uid="{CD364520-9B66-417D-B195-925AAF6E8BA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -423,16 +423,6 @@
 Port map in BTM shows CAN_CLK mapped to i_can_clk</t>
   </si>
   <si>
-    <t>Port map in MCIF shows CAN_CLK mapped to i_can_clk
-Port map in CREG shows CAN_CLK mapped to i_can_clk
-Port map in TX_FIFO shows CAN_CLK mapped to i_can_clk
-Port map in RX_FIFO shows CAN_CLK mapped to i_can_clk
-Port map in TXPL shows CAN_CLK mapped to i_can_clk
-Port map in AFM shows CAN_CLK mapped to i_can_clk
-Port map in BSP shows CAN_CLK mapped to i_can_clk
-Port map in BTM shows CAN_CLK mapped to i_can_clk</t>
-  </si>
-  <si>
     <t>Port map in BTM shows CAN_PHY_RX is mapped to CAN_PHY_RX</t>
   </si>
   <si>
@@ -513,22 +503,6 @@
 Wait until IP2Bus_Ack = 1:</t>
   </si>
   <si>
-    <t>First Clock Cycle:
-IP2Bus_Data = 0x0000_0000
-Second Clock Cycle:
-IP2Bus_Data = 0x0000_0000
-Third Clock Cycle:
-IP2Bus_Data = 0x0000_0000
-Wait until IP2Bus_Ack = 1:
-IP2Bus_Data = 0x0000_0000
-Wait until IP2Bus_Ack = 0:
-IP2Bus_Data = 0x0000_0000
-Wait for one clock cycle:
-IP2Bus_Data = 0x0000_0000
-Wait until IP2Bus_Ack = 1:
-IP2Bus_Data = 0x0000_0000</t>
-  </si>
-  <si>
     <t>1. Set Bus2IP_Reset to 1 for 2 clock cycles
 2. Set Bus2IP_Reset to 0 for one clock cycle
 3. Set Bus2IP_CS to 1 for 2 clock cycles
@@ -769,48 +743,6 @@
   </si>
   <si>
     <t>Sequential write operation occur only if Bus2IP_CS is toggled 0 to 1 or Bus2IP_RNW goes from 1 to 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">After reset:
-Bus2IP_Addr = 0x24
-Bus2IP_Data = 0xAAAA_AAAA
-Bus2IP_RNW = 1
-Bus2IP_CS = 1
-when IP2Bus_Ack = 1:
-After IP2Bus_Ack = 0:
-Bus2IP_RNW = 1
-When IP2Bus_Ack = 1:
-After IP2Bus_Ack is set to 0:
-After 2 Clock cycles:
-After toggling the Bus2IP_CS:
-When IP2Bus_Ack = 1:
-</t>
-  </si>
-  <si>
-    <t>After reset:
-IP2Bus_Data = 0x0000_0000
-IP2Bus_Ack = 0
-When IP2Bus_Ack = 1:
-IP2Bus_Data = 0x0000_0000
-IP2Bus_Ack = 1
-After IP2Bus_Ack = 0:
-IP2Bus_Data = 0x0000_0000
-IP2Bus_Ack = 0
-When IP2Bus_Ack = 1:
-IP2Bus_Data = 0xAAAA_AAAA
-IP2Bus_Ack = 1
-After IP2Bus_Ack is set to 0:
-IP2Bus_Data = 0x0000_0000
-IP2Bus_Ack = 0
-After 2 Clock Cycles:
-IP2Bus_Data = 0x0000_0000
-IP2Bus_Ack = 0
-After toggling Bus2IP_CS:
-IP2Bus_Data = 0x0000_0000
-IP2Bus_Ack = 0
-When IP2Bus_Ack = 1:
-IP2Bus_Data = 0xAAAA_AAAA
-IP2Bus_Ack = 1</t>
   </si>
   <si>
     <t>Sequential Read operation occur only if Bus2IP_CS is toggled 0 to 1 or Bus2IP_RNW goes from 0 to 1</t>
@@ -831,23 +763,6 @@
 13. Set Bus2IP_CS to 1
 14. Wait until IP2Bus_Ack is set to 1
 15. Observe 0xBBBB_BBBB written to address 0x24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Set Bus2IP_Reset to 1 for 2 clock cycles
-2. Set Bus2IP_Addr to 0x24, Bus2IP_Data to 0xAAAA_AAAA, Bus2IP_RNW to 0, and Bus2IP_CS to 1
-3. Set Bus2IP_Reset to 0 and wait for IP2Bus_Ack to be 1
-4. Wait till IP2Bus_Ack is set to 0
-5. Set Bus2IP_RNW to 1
-6. Wait until IP2Bus_Ack is set to 1
-7. Observe IP2Bus_Data is 0xAAAA_AAAA
-8. Wait until IP2Bus_Ack is set to 0
-9. Wait for 2 clock cycles
-10. Observe IP2Bus_Data is 0x0000_0000 and IP2Bus_Ack is 0
-11. Set Bus2IP_CS to 0 for one clock cycle
-12. Set Bus2IP_CS to 1
-13. Wait until IP2Bus_Ack is set to 1
-14. Observe IP2Bus_data is 0xAAAA_AAAA
-</t>
   </si>
   <si>
     <t xml:space="preserve">After reset:
@@ -891,6 +806,100 @@
 When IP2Bus_Ack = 1:
 IP2Bus_Data = 0xBBBB_BBBB
 IP2Bus_Ack = 1</t>
+  </si>
+  <si>
+    <t>Port map in MCIF shows CAN_CLK mapped to i_can_clk
+Port map in CREG shows CAN_CLK mapped to i_can_clk
+Port map in TX_FIFO shows CAN_CLK mapped to i_can_clk
+Port map in RX_FIFO shows CAN_CLK mapped to i_can_clk
+Port map in TXPL shows CAN_CLK mapped to i_can_clk
+Port map in AFM shows CAN_CLK mapped to i_can_clk</t>
+  </si>
+  <si>
+    <t>First Clock Cycle:
+IP2Bus_Data = 0x0000_0000
+Second Clock Cycle:
+IP2Bus_Data = 0x0000_0000
+Third Clock Cycle:
+IP2Bus_Data = 0x0000_0000
+Wait until IP2Bus_Ack = 1:
+IP2Bus_Data = 0x0000_0000
+Wait until IP2Bus_Ack = 0:
+IP2Bus_Data = 0x0000_0000
+Wait for one clock cycle:
+IP2Bus_Data = 0x0000_0000
+Wait until IP2Bus_Ack = 1:
+IP2Bus_Data = 0xAAAA_AAAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set Bus2IP_Reset to 1 for 2 clock cycles
+2. Set Bus2IP_Addr to 0x24, Bus2IP_Data to 0xAAAA_AAAA, Bus2IP_RNW to 0, and Bus2IP_CS to 1
+3. Set Bus2IP_Reset to 0 and wait for IP2Bus_Ack to be 1
+4. Wait till IP2Bus_Ack is set to 0
+5. Set Bus2IP_RNW to 1
+6. Wait until IP2Bus_Ack is set to 1
+7. Observe IP2Bus_Data is 0xAAAA_AAAA
+8. Wait until IP2Bus_Ack is set to 0
+9. Wait for 2 clock cycles
+10. Observe IP2Bus_Data is 0x0000_0000 and IP2Bus_Ack is 0
+11. Set Bus2IP_CS to 0 for one clock cycle
+12. Set Bus2IP_CS to 1
+13. Wait until IP2Bus_Ack is set to 1
+14. Observe IP2Bus_data is 0xAAAA_AAAA
+15. Wait for 2 clock cycles
+16 Observe IP2Bus_data is 0xAAAA_AAAA
+17. Set Bus2IP_CS to 0
+18.Observe IP2Bus_Data is 0x0000_0000
+</t>
+  </si>
+  <si>
+    <t>After reset:
+Bus2IP_Addr = 0x24
+Bus2IP_Data = 0xAAAA_AAAA
+Bus2IP_RNW = 1
+Bus2IP_CS = 1
+when IP2Bus_Ack = 1:
+After IP2Bus_Ack = 0:
+Bus2IP_RNW = 1
+When IP2Bus_Ack = 1:
+After IP2Bus_Ack is set to 0:
+After 2 Clock cycles:
+After toggling the Bus2IP_CS:
+When IP2Bus_Ack = 1:
+After 2 clock cycles:
+After Bus2IP_CS is set to 0:</t>
+  </si>
+  <si>
+    <t>After reset:
+IP2Bus_Data = 0x0000_0000
+IP2Bus_Ack = 0
+When IP2Bus_Ack = 1:
+IP2Bus_Data = 0x0000_0000
+IP2Bus_Ack = 1
+After IP2Bus_Ack = 0:
+IP2Bus_Data = 0x0000_0000
+IP2Bus_Ack = 0
+When IP2Bus_Ack = 1:
+IP2Bus_Data = 0xAAAA_AAAA
+IP2Bus_Ack = 1
+After IP2Bus_Ack is set to 0:
+IP2Bus_Data = 0x0000_0000
+IP2Bus_Ack = 0
+After 2 Clock Cycles:
+IP2Bus_Data = 0x0000_0000
+IP2Bus_Ack = 0
+After toggling Bus2IP_CS:
+IP2Bus_Data = 0x0000_0000
+IP2Bus_Ack = 0
+When IP2Bus_Ack = 1:
+IP2Bus_Data = 0xAAAA_AAAA
+IP2Bus_Ack = 1
+After 2 clock cycles:
+IP2Bus_Data = 0xAAAA_AAAA
+IP2Bus_Ack = 0
+After Bus2IP_CS is set to 0:
+IP2Bus_Data = 0x0000_0000
+IP2Bus_Ack = 0</t>
   </si>
 </sst>
 </file>
@@ -1263,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D5DC9A-6377-4D85-82E7-1C9EAFEEE72B}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="D25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,19 +1486,19 @@
         <v>49</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D10" t="s">
-        <v>169</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1506,7 +1515,7 @@
         <v>91</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>127</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1546,7 +1555,7 @@
         <v>91</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1566,7 +1575,7 @@
         <v>91</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1604,7 +1613,7 @@
         <v>91</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1624,7 +1633,7 @@
         <v>91</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1644,7 +1653,7 @@
         <v>91</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1664,7 +1673,7 @@
         <v>91</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1684,7 +1693,7 @@
         <v>91</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1704,7 +1713,7 @@
         <v>91</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1724,15 +1733,15 @@
         <v>91</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>111</v>
@@ -1744,7 +1753,7 @@
         <v>91</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="330" x14ac:dyDescent="0.25">
@@ -1755,19 +1764,19 @@
         <v>62</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>144</v>
-      </c>
       <c r="F24" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -1775,16 +1784,16 @@
         <v>63</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
@@ -1795,16 +1804,16 @@
         <v>64</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>188</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1815,16 +1824,16 @@
         <v>65</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E27" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="210" x14ac:dyDescent="0.25">
@@ -1835,19 +1844,19 @@
         <v>66</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D28" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:6" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
@@ -1855,16 +1864,16 @@
         <v>67</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
@@ -1875,16 +1884,16 @@
         <v>68</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1895,16 +1904,16 @@
         <v>69</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1915,16 +1924,16 @@
         <v>70</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1935,16 +1944,16 @@
         <v>71</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="F33" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="270" x14ac:dyDescent="0.25">
@@ -1955,16 +1964,16 @@
         <v>72</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -1975,16 +1984,16 @@
         <v>73</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="195" x14ac:dyDescent="0.25">
@@ -1995,16 +2004,16 @@
         <v>74</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="E36" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CAN1-78 Addressed v2 Comments for Top Module Test Cases --Antonio
</commit_message>
<xml_diff>
--- a/Documentations/Test Cases/top_module_test_cases.xlsx
+++ b/Documentations/Test Cases/top_module_test_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\God\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C644C21-2CE2-4D86-9F9E-0F213629FF9B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816339BE-93CC-419B-A277-ACE65E1B78FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8070" yWindow="4665" windowWidth="17055" windowHeight="11385" xr2:uid="{CD364520-9B66-417D-B195-925AAF6E8BA3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD364520-9B66-417D-B195-925AAF6E8BA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="192">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -740,12 +740,6 @@
 IP2Bus_IntrEvent = 0
 When IP2Bus_Ack is 1:
 IP2Bus_IntrEvent = 0</t>
-  </si>
-  <si>
-    <t>Sequential write operation occur only if Bus2IP_CS is toggled 0 to 1 or Bus2IP_RNW goes from 1 to 0</t>
-  </si>
-  <si>
-    <t>Sequential Read operation occur only if Bus2IP_CS is toggled 0 to 1 or Bus2IP_RNW goes from 0 to 1</t>
   </si>
   <si>
     <t>1. Set Bus2IP_Reset to 1 for 2 clock cycles
@@ -808,14 +802,6 @@
 IP2Bus_Ack = 1</t>
   </si>
   <si>
-    <t>Port map in MCIF shows CAN_CLK mapped to i_can_clk
-Port map in CREG shows CAN_CLK mapped to i_can_clk
-Port map in TX_FIFO shows CAN_CLK mapped to i_can_clk
-Port map in RX_FIFO shows CAN_CLK mapped to i_can_clk
-Port map in TXPL shows CAN_CLK mapped to i_can_clk
-Port map in AFM shows CAN_CLK mapped to i_can_clk</t>
-  </si>
-  <si>
     <t>First Clock Cycle:
 IP2Bus_Data = 0x0000_0000
 Second Clock Cycle:
@@ -832,74 +818,93 @@
 IP2Bus_Data = 0xAAAA_AAAA</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Set Bus2IP_Reset to 1 for 2 clock cycles
+    <t>Port map in MCIF shows CAN_CLK mapped to i_sys_clk
+Port map in CREG shows CAN_CLK mapped to i_sys_clk
+Port map in TX_FIFO shows CAN_CLK mapped to i_sys_clk
+Port map in RX_FIFO shows CAN_CLK mapped to i_sys_clk
+Port map in TXPL shows CAN_CLK mapped to i_sys_clk
+Port map in AFM shows CAN_CLK mapped to i_sys_clk</t>
+  </si>
+  <si>
+    <t>Sequential read operation occur only if Bus2IP_CS is toggled 0 to 1</t>
+  </si>
+  <si>
+    <t>Sequential write operation occur only if Bus2IP_CS is toggled 0 to 1</t>
+  </si>
+  <si>
+    <t>Mapping of int_reset to Bus2IP_Reset and CREG o_soft_reset or'd
+exists</t>
+  </si>
+  <si>
+    <t>1. Set Bus2IP_Reset to 1 for 2 clock cycles
 2. Set Bus2IP_Addr to 0x24, Bus2IP_Data to 0xAAAA_AAAA, Bus2IP_RNW to 0, and Bus2IP_CS to 1
 3. Set Bus2IP_Reset to 0 and wait for IP2Bus_Ack to be 1
 4. Wait till IP2Bus_Ack is set to 0
-5. Set Bus2IP_RNW to 1
-6. Wait until IP2Bus_Ack is set to 1
-7. Observe IP2Bus_Data is 0xAAAA_AAAA
+5. Set Bus2IP_CS to 0 for one clock cycle
+6. Set Bus2IP_CS to 1, Bus2IP_Data to 0xBBBB_BBBB, and Bus2IP_Addr to 0x28
+7. Wait until IP2Bus_Ack is set to 1
 8. Wait until IP2Bus_Ack is set to 0
-9. Wait for 2 clock cycles
-10. Observe IP2Bus_Data is 0x0000_0000 and IP2Bus_Ack is 0
-11. Set Bus2IP_CS to 0 for one clock cycle
-12. Set Bus2IP_CS to 1
-13. Wait until IP2Bus_Ack is set to 1
-14. Observe IP2Bus_data is 0xAAAA_AAAA
-15. Wait for 2 clock cycles
-16 Observe IP2Bus_data is 0xAAAA_AAAA
-17. Set Bus2IP_CS to 0
-18.Observe IP2Bus_Data is 0x0000_0000
-</t>
-  </si>
-  <si>
-    <t>After reset:
+9. Set Bus2IP_RNW to 1 and Bus2IP_Addr to 0x24
+10. Wait until IP2Bus_Ack is set to 1
+11. Observe IP2Bus_Data is 0xAAAA_AAAA
+12. Set Bus2IP_Addr to 0x28
+13. Wait for 3 clock cycles
+14. Observe that IP2Bus_Data is 0xAAAA_AAAA
+15. Set Bus2IP_CS to 0 for one clock cycle
+16. Set Bus2IP_CS to 1
+17 Wait until IP2Bus_Ack is set to 1
+18. Observe that IP2Bus_Data is 0xBBBB_BBBB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After reset:
 Bus2IP_Addr = 0x24
 Bus2IP_Data = 0xAAAA_AAAA
 Bus2IP_RNW = 1
 Bus2IP_CS = 1
 when IP2Bus_Ack = 1:
 After IP2Bus_Ack = 0:
-Bus2IP_RNW = 1
+Bus2IP_CS = 0
+After 1 clock cycle:
+BUS2IP_CS = 1
+Bus2IP_Data = 0xBBBB_BBBB
+Bus2IP_Addr = 0x28
 When IP2Bus_Ack = 1:
 After IP2Bus_Ack is set to 0:
-After 2 Clock cycles:
-After toggling the Bus2IP_CS:
-When IP2Bus_Ack = 1:
-After 2 clock cycles:
-After Bus2IP_CS is set to 0:</t>
+Bus2IP_RNW = 1
+Bus2IP_Addr = 0x24
+when IP2Bus_ack = 1:
+After IP2Bus_Ack = 0:
+Bus2IP_Addr = 0x28
+After 3 clock cycles:
+Bus2IP_CS = 0
+After 1 clock cycle:
+Bus2IP_CS = 1
+when IP2Bus_Ack = 1
+</t>
   </si>
   <si>
     <t>After reset:
 IP2Bus_Data = 0x0000_0000
-IP2Bus_Ack = 0
 When IP2Bus_Ack = 1:
 IP2Bus_Data = 0x0000_0000
-IP2Bus_Ack = 1
 After IP2Bus_Ack = 0:
 IP2Bus_Data = 0x0000_0000
-IP2Bus_Ack = 0
+After 1 clock cycle:
+IP2Bus_Data = 0x0000_0000
 When IP2Bus_Ack = 1:
-IP2Bus_Data = 0xAAAA_AAAA
-IP2Bus_Ack = 1
+IP2Bus_Data = 0x0000_0000
 After IP2Bus_Ack is set to 0:
 IP2Bus_Data = 0x0000_0000
-IP2Bus_Ack = 0
-After 2 Clock Cycles:
-IP2Bus_Data = 0x0000_0000
-IP2Bus_Ack = 0
-After toggling Bus2IP_CS:
-IP2Bus_Data = 0x0000_0000
-IP2Bus_Ack = 0
+When IP2Bus_Ack = 1
+IP2Bus_Data = 0xAAAA_AAAA
+After IP2Bus_Ack = 0:
+IP2Bus_Data = 0xAAAA_AAAA
+After 3 clock cycles:
+IP2Bus_Data = 0xAAAA_AAAA
+After 1 clock cycle:
+IP2Bus_Data = 0xAAAA_AAAA
 When IP2Bus_Ack = 1:
-IP2Bus_Data = 0xAAAA_AAAA
-IP2Bus_Ack = 1
-After 2 clock cycles:
-IP2Bus_Data = 0xAAAA_AAAA
-IP2Bus_Ack = 0
-After Bus2IP_CS is set to 0:
-IP2Bus_Data = 0x0000_0000
-IP2Bus_Ack = 0</t>
+IP2Bus_Data = 0xBBBB_BBBB</t>
   </si>
 </sst>
 </file>
@@ -929,12 +934,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -949,11 +960,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1270,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D5DC9A-6377-4D85-82E7-1C9EAFEEE72B}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,8 +1538,8 @@
       <c r="E11" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>186</v>
+      <c r="F11" s="4" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1538,7 +1562,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1594,7 +1618,9 @@
       <c r="E15" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="4" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1773,10 +1799,10 @@
         <v>143</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="192" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -1796,244 +1822,275 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="1" customFormat="1" ht="189" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:6" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="210" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="E31" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="F31" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    </row>
+    <row r="32" spans="1:6" s="1" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F33" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F35" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="270" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="36" spans="1:6" ht="270" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F36" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="37" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F37" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="195" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="38" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CAN1-78 Made Requested Changes to Top Module Test Cases --Antonio
</commit_message>
<xml_diff>
--- a/Documentations/Test Cases/top_module_test_cases.xlsx
+++ b/Documentations/Test Cases/top_module_test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\God\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816339BE-93CC-419B-A277-ACE65E1B78FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D903F5C5-1269-4EB5-807C-C5C44B1A13E9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD364520-9B66-417D-B195-925AAF6E8BA3}"/>
   </bookViews>
@@ -776,32 +776,6 @@
 </t>
   </si>
   <si>
-    <t>After reset:
-Register at address 0x24 = 0x0000_0000
-IP2Bus_Ack = 0
-When IP2Bus_Ack = 1:
-Register at address 0x24 = 0x0000_0000
-IP2Bus_Ack = 1
-After IP2Bus_Ack = 0:
-Register at address 0x24 = 0x0000_0000
-IP2Bus_Ack = 0
-When IP2Bus_Ack = 1:
-Register at address 0x24 = 0xAAAA_AAAA
-IP2Bus_Ack = 1
-After IP2Bus_Ack is set to 0:
-Register at address 0x24 = 0xAAAA_AAAA
-IP2Bus_Ack = 0
-After 2 Clock Cycles:
-Register at address 0x24 = 0xAAAA_AAAA
-IP2Bus_Ack = 0
-After toggling Bus2IP_CS:
-Register at address 0x24 = 0xAAAA_AAAA
-IP2Bus_Ack = 0
-When IP2Bus_Ack = 1:
-IP2Bus_Data = 0xBBBB_BBBB
-IP2Bus_Ack = 1</t>
-  </si>
-  <si>
     <t>First Clock Cycle:
 IP2Bus_Data = 0x0000_0000
 Second Clock Cycle:
@@ -816,14 +790,6 @@
 IP2Bus_Data = 0x0000_0000
 Wait until IP2Bus_Ack = 1:
 IP2Bus_Data = 0xAAAA_AAAA</t>
-  </si>
-  <si>
-    <t>Port map in MCIF shows CAN_CLK mapped to i_sys_clk
-Port map in CREG shows CAN_CLK mapped to i_sys_clk
-Port map in TX_FIFO shows CAN_CLK mapped to i_sys_clk
-Port map in RX_FIFO shows CAN_CLK mapped to i_sys_clk
-Port map in TXPL shows CAN_CLK mapped to i_sys_clk
-Port map in AFM shows CAN_CLK mapped to i_sys_clk</t>
   </si>
   <si>
     <t>Sequential read operation occur only if Bus2IP_CS is toggled 0 to 1</t>
@@ -905,6 +871,40 @@
 IP2Bus_Data = 0xAAAA_AAAA
 When IP2Bus_Ack = 1:
 IP2Bus_Data = 0xBBBB_BBBB</t>
+  </si>
+  <si>
+    <t>Port map in MCIF shows SYS_CLK mapped to i_sys_clk
+Port map in CREG shows SYS_CLK mapped to i_sys_clk
+Port map in TX_FIFO shows SYS_CLK mapped to i_sys_clk
+Port map in RX_FIFO shows SYS_CLK mapped to i_sys_clk
+Port map in TXPL shows SYS_CLK mapped to i_sys_clk
+Port map in AFM shows SYS_CLK mapped to i_sys_clk</t>
+  </si>
+  <si>
+    <t>After reset:
+Register at address 0x24 = 0x0000_0000
+IP2Bus_Ack = 0
+When IP2Bus_Ack = 1:
+Register at address 0x24 = 0x0000_0000
+IP2Bus_Ack = 1
+After IP2Bus_Ack = 0:
+Register at address 0x24 = 0x0000_0000
+IP2Bus_Ack = 0
+When IP2Bus_Ack = 1:
+Register at address 0x24 = 0xAAAA_AAAA
+IP2Bus_Ack = 1
+After IP2Bus_Ack is set to 0:
+Register at address 0x24 = 0xAAAA_AAAA
+IP2Bus_Ack = 0
+After 2 Clock Cycles:
+Register at address 0x24 = 0xAAAA_AAAA
+IP2Bus_Ack = 0
+After toggling Bus2IP_CS:
+Register at address 0x24 = 0xAAAA_AAAA
+IP2Bus_Ack = 0
+When IP2Bus_Ack = 1:
+Register at address 0x24 = 0xBBBB_BBBB
+IP2Bus_Ack = 1</t>
   </si>
 </sst>
 </file>
@@ -970,12 +970,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1296,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D5DC9A-6377-4D85-82E7-1C9EAFEEE72B}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1539,7 +1539,7 @@
         <v>91</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1619,7 +1619,7 @@
         <v>91</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -1799,7 +1799,7 @@
         <v>143</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="192" customHeight="1" x14ac:dyDescent="0.25">
@@ -1823,31 +1823,31 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="D26" s="7" t="s">
+      <c r="C26" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>191</v>
-      </c>
     </row>
     <row r="27" spans="1:6" s="1" customFormat="1" ht="189" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:6" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1911,32 +1911,32 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="D31" s="7" t="s">
+      <c r="C31" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="F31" s="7" t="s">
-        <v>183</v>
+      <c r="F31" s="6" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="1" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -2076,11 +2076,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
     <mergeCell ref="F31:F32"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="B26:B27"/>
@@ -2088,6 +2083,11 @@
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="F26:F27"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>